<commit_message>
Define Setup TC script completed
</commit_message>
<xml_diff>
--- a/VRT/TestData/SetupTestData.xlsx
+++ b/VRT/TestData/SetupTestData.xlsx
@@ -8,13 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manoj.ghadei\git\VRT\VRT\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F15C093-AC62-4069-BB52-9E4B19D2C0CD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA9F743F-DBAE-414B-9120-03E3A4A7A13C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="847" activeTab="1" xr2:uid="{88CC17F3-0530-4FB5-9C07-02E67965A03F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="847" activeTab="8" xr2:uid="{88CC17F3-0530-4FB5-9C07-02E67965A03F}"/>
   </bookViews>
   <sheets>
-    <sheet name="SET019a" sheetId="2" r:id="rId1"/>
-    <sheet name="SET019b" sheetId="1" r:id="rId2"/>
+    <sheet name="SET019" sheetId="2" r:id="rId1"/>
+    <sheet name="SET020" sheetId="1" r:id="rId2"/>
+    <sheet name="SET024" sheetId="3" r:id="rId3"/>
+    <sheet name="SET025" sheetId="4" r:id="rId4"/>
+    <sheet name="SET026a" sheetId="5" r:id="rId5"/>
+    <sheet name="SET026b" sheetId="6" r:id="rId6"/>
+    <sheet name="SET027a" sheetId="7" r:id="rId7"/>
+    <sheet name="SET027b" sheetId="8" r:id="rId8"/>
+    <sheet name="SET028" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -24,6 +31,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="82">
   <si>
     <t xml:space="preserve">  </t>
   </si>
@@ -148,6 +156,135 @@
   </si>
   <si>
     <t>Setup Name accepts alpha numeric and special characters like -_  and :</t>
+  </si>
+  <si>
+    <t>299</t>
+  </si>
+  <si>
+    <t>300</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>-1</t>
+  </si>
+  <si>
+    <t>@</t>
+  </si>
+  <si>
+    <t>`</t>
+  </si>
+  <si>
+    <t>~</t>
+  </si>
+  <si>
+    <t>!</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>$</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>^</t>
+  </si>
+  <si>
+    <t>&amp;</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>()</t>
+  </si>
+  <si>
+    <t>|</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>=</t>
+  </si>
+  <si>
+    <t>{}</t>
+  </si>
+  <si>
+    <t>"</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>;</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>,</t>
+  </si>
+  <si>
+    <t>&lt;&gt;</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>_</t>
+  </si>
+  <si>
+    <t>:</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>Number of Sensors is mandatory, please enter Number of Sensors</t>
+  </si>
+  <si>
+    <t>123456789012345678901234567890123456789012345678901</t>
+  </si>
+  <si>
+    <t>SOP</t>
+  </si>
+  <si>
+    <t>a\</t>
+  </si>
+  <si>
+    <t>a/</t>
+  </si>
+  <si>
+    <t>SOP Protocol Number accepts alpha numeric and special characters like -,_ ,slash (forward and backward).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     </t>
+  </si>
+  <si>
+    <t>LoadDescription</t>
+  </si>
+  <si>
+    <t>Load Description accepts alpha numeric and special characters like -,_ ,slash (forward and backward).</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>@`~!#$%^&amp;*()|+={}"[]`;?</t>
+  </si>
+  <si>
+    <t>,&lt;&gt;:A2-_\/.a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        </t>
   </si>
 </sst>
 </file>
@@ -191,7 +328,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -199,17 +336,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -533,7 +690,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A3" sqref="A3:A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -632,10 +789,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F772A9F6-A3B5-402F-8C68-9034BA270367}">
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
+      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -913,4 +1070,1147 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{014BDF4D-CBB5-4F9C-BB9D-27B4EA7688A0}">
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3299206D-8880-48B7-8144-E8CD00C5D1F6}">
+  <dimension ref="A1:B29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="60.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AE30440-E635-4D52-A1CC-D1E4951C2625}">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DDC6971-A18E-444E-9493-5CE9E01DA64C}">
+  <dimension ref="A1:C24"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="3" max="3" width="96.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EE32352-9683-412A-B278-9DA687CA0934}">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E2AD9DE-E990-4788-8991-F092345FE2E6}">
+  <dimension ref="A1:C24"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="96.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{877B8675-5E30-4B61-969A-02BF4D248B77}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>